<commit_message>
updated status of reinsurance tests
</commit_message>
<xml_diff>
--- a/validation/examples/reinsurance_test_case_list.xlsx
+++ b/validation/examples/reinsurance_test_case_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\validation\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F338F43F-B1E1-4D21-A22F-0B51DA3388FC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03778BF-EBA6-450B-A5AB-0EE9A8A709BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1152" windowWidth="23040" windowHeight="8964" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="27">
   <si>
     <t>FolderName</t>
   </si>
@@ -113,7 +113,7 @@
     <t>complete</t>
   </si>
   <si>
-    <t>test</t>
+    <t>in progress</t>
   </si>
 </sst>
 </file>
@@ -508,8 +508,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
   <dimension ref="A1:M153"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A138" workbookViewId="0">
-      <selection activeCell="E152" sqref="E152"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -628,7 +628,7 @@
         <v>22</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
@@ -754,7 +754,7 @@
         <v>22</v>
       </c>
       <c r="M7" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
@@ -788,7 +788,7 @@
         <v>22</v>
       </c>
       <c r="M8" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
@@ -920,7 +920,7 @@
         <v>22</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
@@ -1043,7 +1043,7 @@
         <v>22</v>
       </c>
       <c r="M16" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
@@ -1071,8 +1071,8 @@
       <c r="L17" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="M17" s="1" t="s">
-        <v>26</v>
+      <c r="M17" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
@@ -1106,7 +1106,7 @@
         <v>22</v>
       </c>
       <c r="M18" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
@@ -1232,6 +1232,9 @@
       <c r="L22" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M22" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
@@ -1389,6 +1392,9 @@
       </c>
       <c r="L27" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.3">
@@ -1419,6 +1425,9 @@
       <c r="L28" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M28" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
@@ -1503,6 +1512,9 @@
       <c r="L31" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M31" s="2" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
@@ -1535,7 +1547,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_32</v>
@@ -1565,8 +1577,11 @@
       <c r="L33" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M33" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_33</v>
@@ -1597,7 +1612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_34</v>
@@ -1628,7 +1643,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_35</v>
@@ -1659,7 +1674,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_36</v>
@@ -1689,8 +1704,11 @@
       <c r="L37" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M37" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_37</v>
@@ -1717,8 +1735,11 @@
       <c r="L38" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M38" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_38</v>
@@ -1750,8 +1771,11 @@
       <c r="L39" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M39" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_39</v>
@@ -1784,7 +1808,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>QS12_40</v>
@@ -1817,7 +1841,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_41</v>
@@ -1846,7 +1870,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_42</v>
@@ -1874,8 +1898,11 @@
       <c r="L43" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M43" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_43</v>
@@ -1904,7 +1931,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_44</v>
@@ -1929,8 +1956,11 @@
       <c r="L45" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M45" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_45</v>
@@ -1961,7 +1991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_46</v>
@@ -1992,7 +2022,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_47</v>
@@ -2022,8 +2052,11 @@
       <c r="L48" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M48" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_48</v>
@@ -2053,8 +2086,11 @@
       <c r="L49" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M49" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_49</v>
@@ -2085,7 +2121,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_50</v>
@@ -2116,7 +2152,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_51</v>
@@ -2149,7 +2185,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_52</v>
@@ -2181,8 +2217,11 @@
       <c r="L53" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M53" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_53</v>
@@ -2215,7 +2254,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_54</v>
@@ -2246,7 +2285,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_55</v>
@@ -2277,7 +2316,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_56</v>
@@ -2307,8 +2346,11 @@
       <c r="L57" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M57" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_57</v>
@@ -2335,8 +2377,11 @@
       <c r="L58" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M58" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_58</v>
@@ -2368,8 +2413,11 @@
       <c r="L59" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M59" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_59</v>
@@ -2402,7 +2450,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="str">
         <f t="shared" si="0"/>
         <v>PR18_60</v>
@@ -2435,7 +2483,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_61</v>
@@ -2468,7 +2516,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_62</v>
@@ -2500,8 +2548,11 @@
       <c r="L63" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M63" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_63</v>
@@ -2534,7 +2585,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_64</v>
@@ -2569,7 +2620,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_65</v>
@@ -2604,7 +2655,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="str">
         <f t="shared" ref="A67:A130" si="1">LEFT(D67,2)&amp;TEXT(C67,"00")&amp;"_"&amp;B67</f>
         <v>PR20_66</v>
@@ -2638,8 +2689,11 @@
       <c r="L67" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M67" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_67</v>
@@ -2667,8 +2721,11 @@
       <c r="L68" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M68" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_68</v>
@@ -2697,7 +2754,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_69</v>
@@ -2726,7 +2783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_70</v>
@@ -2752,7 +2809,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_71</v>
@@ -2783,7 +2840,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_72</v>
@@ -2813,8 +2870,11 @@
       <c r="L73" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M73" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_73</v>
@@ -2845,7 +2905,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_74</v>
@@ -2876,7 +2936,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_75</v>
@@ -2907,7 +2967,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_76</v>
@@ -2937,8 +2997,11 @@
       <c r="L77" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M77" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_77</v>
@@ -2970,8 +3033,11 @@
       <c r="L78" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M78" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_78</v>
@@ -3004,7 +3070,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_79</v>
@@ -3037,7 +3103,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_80</v>
@@ -3068,7 +3134,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_81</v>
@@ -3098,8 +3164,11 @@
       <c r="L82" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M82" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_82</v>
@@ -3130,7 +3199,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_83</v>
@@ -3157,8 +3226,11 @@
       <c r="L84" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M84" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_84</v>
@@ -3191,7 +3263,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_85</v>
@@ -3224,7 +3296,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="str">
         <f t="shared" si="1"/>
         <v>PR26_86</v>
@@ -3256,8 +3328,11 @@
       <c r="L87" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M87" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_87</v>
@@ -3289,8 +3364,11 @@
       <c r="L88" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M88" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_88</v>
@@ -3323,7 +3401,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_89</v>
@@ -3356,7 +3434,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_90</v>
@@ -3391,7 +3469,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_91</v>
@@ -3425,8 +3503,11 @@
       <c r="L92" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M92" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>PR28_92</v>
@@ -3461,7 +3542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_93</v>
@@ -3490,7 +3571,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_94</v>
@@ -3519,7 +3600,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_95</v>
@@ -3547,8 +3628,11 @@
       <c r="L96" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M96" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_96</v>
@@ -3573,8 +3657,11 @@
       <c r="L97" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M97" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_97</v>
@@ -3604,8 +3691,11 @@
       <c r="L98" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M98" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_98</v>
@@ -3636,7 +3726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_99</v>
@@ -3667,7 +3757,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_100</v>
@@ -3694,8 +3784,11 @@
       <c r="L101" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M101" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_101</v>
@@ -3726,7 +3819,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_102</v>
@@ -3756,8 +3849,11 @@
       <c r="L103" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M103" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_103</v>
@@ -3788,7 +3884,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_104</v>
@@ -3815,8 +3911,11 @@
       <c r="L105" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M105" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_105</v>
@@ -3849,7 +3948,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_106</v>
@@ -3882,7 +3981,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_107</v>
@@ -3914,8 +4013,11 @@
       <c r="L108" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M108" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_108</v>
@@ -3944,8 +4046,11 @@
       <c r="L109" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M109" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_109</v>
@@ -3973,8 +4078,11 @@
       <c r="L110" s="1" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="M110" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_110</v>
@@ -4003,7 +4111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_111</v>
@@ -4057,6 +4165,9 @@
       <c r="L113" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M113" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="str">
@@ -4119,6 +4230,9 @@
       <c r="L115" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M115" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="str">
@@ -4178,6 +4292,9 @@
       <c r="L117" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M117" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="118" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="str">
@@ -4271,6 +4388,9 @@
       <c r="L120" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M120" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="121" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="str">
@@ -4299,6 +4419,9 @@
       <c r="L121" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M121" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="str">
@@ -4332,6 +4455,9 @@
       <c r="L122" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="M122" s="2" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="str">
@@ -4428,6 +4554,9 @@
       <c r="K125" s="6"/>
       <c r="L125" s="1" t="s">
         <v>22</v>
+      </c>
+      <c r="M125" s="2" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
changed location of CondPriority field
</commit_message>
<xml_diff>
--- a/validation/examples/reinsurance_test_case_list.xlsx
+++ b/validation/examples/reinsurance_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF\validation\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\OasisLMF\validation\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D03778BF-EBA6-450B-A5AB-0EE9A8A709BB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A4EEFC-25E0-42D7-BF07-19468E48076F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -506,30 +506,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:N153"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M1" sqref="M1"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="B1" sqref="B1"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.88671875" style="1"/>
+    <col min="11" max="11" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.7109375" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -570,7 +573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="str">
         <f>LEFT(D2,2)&amp;TEXT(C2,"00")&amp;"_"&amp;B2</f>
         <v>SS01_1</v>
@@ -599,7 +602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A66" si="0">LEFT(D3,2)&amp;TEXT(C3,"00")&amp;"_"&amp;B3</f>
         <v>SS01_2</v>
@@ -630,8 +633,9 @@
       <c r="M3" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS01_3</v>
@@ -660,7 +664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_4</v>
@@ -692,7 +696,7 @@
       </c>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_5</v>
@@ -723,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_6</v>
@@ -756,8 +760,9 @@
       <c r="M7" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_7</v>
@@ -790,8 +795,9 @@
       <c r="M8" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_8</v>
@@ -822,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_9</v>
@@ -854,7 +860,7 @@
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS04_10</v>
@@ -887,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS04_11</v>
@@ -922,8 +928,9 @@
       <c r="M12" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SS04_12</v>
@@ -956,7 +963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_13</v>
@@ -985,7 +992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_14</v>
@@ -1014,7 +1021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_15</v>
@@ -1045,8 +1052,9 @@
       <c r="M16" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_16</v>
@@ -1074,8 +1082,9 @@
       <c r="M17" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_17</v>
@@ -1108,8 +1117,9 @@
       <c r="M18" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_18</v>
@@ -1140,7 +1150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_19</v>
@@ -1171,7 +1181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_20</v>
@@ -1202,7 +1212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_21</v>
@@ -1235,8 +1245,9 @@
       <c r="M22" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N22" s="2"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_22</v>
@@ -1267,7 +1278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_23</v>
@@ -1295,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_24</v>
@@ -1328,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_25</v>
@@ -1361,7 +1372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_26</v>
@@ -1396,8 +1407,9 @@
       <c r="M27" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N27" s="2"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_27</v>
@@ -1428,8 +1440,9 @@
       <c r="M28" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N28" s="2"/>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_28</v>
@@ -1458,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_29</v>
@@ -1487,7 +1500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_30</v>
@@ -1515,8 +1528,9 @@
       <c r="M31" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N31" s="2"/>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_31</v>
@@ -1547,7 +1561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_32</v>
@@ -1580,8 +1594,9 @@
       <c r="M33" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N33" s="2"/>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_33</v>
@@ -1612,7 +1627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_34</v>
@@ -1643,7 +1658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_35</v>
@@ -1674,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_36</v>
@@ -1707,8 +1722,9 @@
       <c r="M37" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N37" s="2"/>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_37</v>
@@ -1738,8 +1754,9 @@
       <c r="M38" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N38" s="2"/>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_38</v>
@@ -1774,8 +1791,9 @@
       <c r="M39" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N39" s="2"/>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_39</v>
@@ -1808,7 +1826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>QS12_40</v>
@@ -1841,7 +1859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_41</v>
@@ -1870,7 +1888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_42</v>
@@ -1901,8 +1919,9 @@
       <c r="M43" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N43" s="2"/>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_43</v>
@@ -1931,7 +1950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_44</v>
@@ -1959,8 +1978,9 @@
       <c r="M45" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N45" s="2"/>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_45</v>
@@ -1991,7 +2011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_46</v>
@@ -2022,7 +2042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_47</v>
@@ -2055,8 +2075,9 @@
       <c r="M48" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N48" s="2"/>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_48</v>
@@ -2089,8 +2110,9 @@
       <c r="M49" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N49" s="2"/>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_49</v>
@@ -2121,7 +2143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_50</v>
@@ -2152,7 +2174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_51</v>
@@ -2185,7 +2207,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_52</v>
@@ -2220,8 +2242,9 @@
       <c r="M53" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N53" s="2"/>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_53</v>
@@ -2254,7 +2277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_54</v>
@@ -2285,7 +2308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_55</v>
@@ -2316,7 +2339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_56</v>
@@ -2349,8 +2372,9 @@
       <c r="M57" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N57" s="2"/>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_57</v>
@@ -2380,8 +2404,9 @@
       <c r="M58" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N58" s="2"/>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_58</v>
@@ -2416,8 +2441,9 @@
       <c r="M59" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N59" s="2"/>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_59</v>
@@ -2450,7 +2476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="str">
         <f t="shared" si="0"/>
         <v>PR18_60</v>
@@ -2483,7 +2509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_61</v>
@@ -2516,7 +2542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_62</v>
@@ -2551,8 +2577,9 @@
       <c r="M63" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N63" s="2"/>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_63</v>
@@ -2585,7 +2612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_64</v>
@@ -2620,7 +2647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_65</v>
@@ -2655,7 +2682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="str">
         <f t="shared" ref="A67:A130" si="1">LEFT(D67,2)&amp;TEXT(C67,"00")&amp;"_"&amp;B67</f>
         <v>PR20_66</v>
@@ -2692,8 +2719,9 @@
       <c r="M67" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N67" s="2"/>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_67</v>
@@ -2724,8 +2752,9 @@
       <c r="M68" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N68" s="2"/>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_68</v>
@@ -2754,7 +2783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_69</v>
@@ -2783,7 +2812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_70</v>
@@ -2809,7 +2838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_71</v>
@@ -2840,7 +2869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_72</v>
@@ -2873,8 +2902,9 @@
       <c r="M73" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="74" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N73" s="2"/>
+    </row>
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_73</v>
@@ -2905,7 +2935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_74</v>
@@ -2936,7 +2966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_75</v>
@@ -2967,7 +2997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_76</v>
@@ -3000,8 +3030,9 @@
       <c r="M77" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="78" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N77" s="2"/>
+    </row>
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_77</v>
@@ -3036,8 +3067,9 @@
       <c r="M78" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="79" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N78" s="2"/>
+    </row>
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_78</v>
@@ -3070,7 +3102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_79</v>
@@ -3103,7 +3135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_80</v>
@@ -3134,7 +3166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_81</v>
@@ -3167,8 +3199,9 @@
       <c r="M82" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="83" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N82" s="2"/>
+    </row>
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_82</v>
@@ -3199,7 +3232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_83</v>
@@ -3229,8 +3262,9 @@
       <c r="M84" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N84" s="2"/>
+    </row>
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_84</v>
@@ -3263,7 +3297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_85</v>
@@ -3296,7 +3330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="9" t="str">
         <f t="shared" si="1"/>
         <v>PR26_86</v>
@@ -3331,8 +3365,9 @@
       <c r="M87" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N87" s="2"/>
+    </row>
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_87</v>
@@ -3367,8 +3402,9 @@
       <c r="M88" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N88" s="2"/>
+    </row>
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_88</v>
@@ -3401,7 +3437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_89</v>
@@ -3434,7 +3470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_90</v>
@@ -3469,7 +3505,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_91</v>
@@ -3506,8 +3542,9 @@
       <c r="M92" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="93" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N92" s="2"/>
+    </row>
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>PR28_92</v>
@@ -3542,7 +3579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_93</v>
@@ -3571,7 +3608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_94</v>
@@ -3600,7 +3637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_95</v>
@@ -3631,8 +3668,9 @@
       <c r="M96" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="97" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N96" s="2"/>
+    </row>
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_96</v>
@@ -3660,8 +3698,9 @@
       <c r="M97" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="98" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N97" s="2"/>
+    </row>
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_97</v>
@@ -3694,8 +3733,9 @@
       <c r="M98" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="99" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N98" s="2"/>
+    </row>
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_98</v>
@@ -3726,7 +3766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_99</v>
@@ -3757,7 +3797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_100</v>
@@ -3787,8 +3827,9 @@
       <c r="M101" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="102" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N101" s="2"/>
+    </row>
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_101</v>
@@ -3819,7 +3860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_102</v>
@@ -3852,8 +3893,9 @@
       <c r="M103" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="104" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N103" s="2"/>
+    </row>
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_103</v>
@@ -3884,7 +3926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_104</v>
@@ -3914,8 +3956,9 @@
       <c r="M105" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="106" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N105" s="2"/>
+    </row>
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_105</v>
@@ -3948,7 +3991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_106</v>
@@ -3981,7 +4024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_107</v>
@@ -4016,8 +4059,9 @@
       <c r="M108" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N108" s="2"/>
+    </row>
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_108</v>
@@ -4049,8 +4093,9 @@
       <c r="M109" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="110" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N109" s="2"/>
+    </row>
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_109</v>
@@ -4082,7 +4127,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="111" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_110</v>
@@ -4111,7 +4156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_111</v>
@@ -4140,7 +4185,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_112</v>
@@ -4169,7 +4214,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="114" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_113</v>
@@ -4200,7 +4245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_114</v>
@@ -4234,7 +4279,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="116" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_115</v>
@@ -4265,7 +4310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_116</v>
@@ -4296,7 +4341,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="118" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_117</v>
@@ -4327,7 +4372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_118</v>
@@ -4358,7 +4403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_119</v>
@@ -4392,7 +4437,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="121" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_120</v>
@@ -4423,7 +4468,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="122" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_121</v>
@@ -4459,7 +4504,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="123" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_122</v>
@@ -4492,7 +4537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="124" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_123</v>
@@ -4525,7 +4570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>CX36_124</v>
@@ -4559,7 +4604,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="126" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_125</v>
@@ -4590,8 +4635,9 @@
       <c r="M126" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="127" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N126" s="2"/>
+    </row>
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_126</v>
@@ -4620,7 +4666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="128" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_127</v>
@@ -4649,7 +4695,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA38_128</v>
@@ -4680,7 +4726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA38_129</v>
@@ -4713,8 +4759,9 @@
       <c r="M130" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="131" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N130" s="2"/>
+    </row>
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="str">
         <f t="shared" ref="A131:A149" si="2">LEFT(D131,2)&amp;TEXT(C131,"00")&amp;"_"&amp;B131</f>
         <v>FA38_130</v>
@@ -4745,7 +4792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_131</v>
@@ -4776,7 +4823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_132</v>
@@ -4807,7 +4854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_133</v>
@@ -4840,8 +4887,9 @@
       <c r="M134" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="135" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N134" s="2"/>
+    </row>
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_134</v>
@@ -4876,8 +4924,9 @@
       <c r="M135" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="136" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N135" s="2"/>
+    </row>
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_135</v>
@@ -4910,7 +4959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_136</v>
@@ -4943,7 +4992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_137</v>
@@ -4972,7 +5021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_138</v>
@@ -5003,8 +5052,9 @@
       <c r="M139" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="140" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N139" s="2"/>
+    </row>
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_139</v>
@@ -5033,7 +5083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_140</v>
@@ -5064,7 +5114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_141</v>
@@ -5095,7 +5145,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_142</v>
@@ -5128,8 +5178,9 @@
       <c r="M143" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="144" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N143" s="2"/>
+    </row>
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_143</v>
@@ -5162,8 +5213,9 @@
       <c r="M144" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="145" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N144" s="2"/>
+    </row>
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_144</v>
@@ -5194,7 +5246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_145</v>
@@ -5225,7 +5277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA44_146</v>
@@ -5258,7 +5310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA44_147</v>
@@ -5293,8 +5345,9 @@
       <c r="M148" s="1" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="149" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="N148" s="2"/>
+    </row>
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149" s="9" t="str">
         <f t="shared" si="2"/>
         <v>FA44_148</v>
@@ -5328,7 +5381,7 @@
       </c>
       <c r="M149" s="9"/>
     </row>
-    <row r="150" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150" s="9" t="str">
         <f t="shared" ref="A150:A152" si="3">LEFT(D150,2)&amp;TEXT(C150,"00")&amp;"_"&amp;B150</f>
         <v>FA45_149</v>
@@ -5360,11 +5413,11 @@
       <c r="L150" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M150" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="151" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M150" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151" s="9" t="str">
         <f t="shared" si="3"/>
         <v>FA45_150</v>
@@ -5396,11 +5449,11 @@
       <c r="L151" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M151" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="152" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M151" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152" s="9" t="str">
         <f t="shared" si="3"/>
         <v>FA45_151</v>
@@ -5432,11 +5485,11 @@
       <c r="L152" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="M152" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="153" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M152" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153" s="9"/>
       <c r="B153" s="9"/>
       <c r="C153" s="9"/>
@@ -5452,7 +5505,6 @@
       <c r="M153" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M152" xr:uid="{7A1F8883-8032-4EF3-8281-54B98DA6D123}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
renamed and add test cases for reins layer logic
</commit_message>
<xml_diff>
--- a/validation/examples/reinsurance_test_case_list.xlsx
+++ b/validation/examples/reinsurance_test_case_list.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\OasisLMF\validation\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4A4EEFC-25E0-42D7-BF07-19468E48076F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD8C81-D4E2-4F91-AB77-0BDD3881E52D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="836" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="31">
   <si>
     <t>FolderName</t>
   </si>
@@ -114,6 +114,18 @@
   </si>
   <si>
     <t>in progress</t>
+  </si>
+  <si>
+    <t>13-19</t>
+  </si>
+  <si>
+    <t>16, 23</t>
+  </si>
+  <si>
+    <t>QS46_x6</t>
+  </si>
+  <si>
+    <t>QS47_x2</t>
   </si>
 </sst>
 </file>
@@ -506,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
-  <dimension ref="A1:N153"/>
+  <dimension ref="A1:N154"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B120" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomRight" activeCell="M154" sqref="M154"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5454,32 +5466,32 @@
       </c>
     </row>
     <row r="152" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A152" s="9" t="str">
+      <c r="A152" s="6" t="str">
         <f t="shared" si="3"/>
         <v>FA45_151</v>
       </c>
-      <c r="B152" s="9">
+      <c r="B152" s="6">
         <v>151</v>
       </c>
-      <c r="C152" s="9">
+      <c r="C152" s="6">
         <v>45</v>
       </c>
-      <c r="D152" s="10" t="s">
+      <c r="D152" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="E152" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F152" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="G152" s="10"/>
-      <c r="H152" s="10"/>
-      <c r="I152" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="J152" s="9"/>
-      <c r="K152" s="9" t="s">
+      <c r="E152" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F152" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" s="8"/>
+      <c r="H152" s="8"/>
+      <c r="I152" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="J152" s="6"/>
+      <c r="K152" s="6" t="s">
         <v>15</v>
       </c>
       <c r="L152" s="9" t="s">
@@ -5490,19 +5502,62 @@
       </c>
     </row>
     <row r="153" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A153" s="9"/>
-      <c r="B153" s="9"/>
-      <c r="C153" s="9"/>
-      <c r="D153" s="10"/>
-      <c r="E153" s="9"/>
+      <c r="A153" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="B153" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="C153" s="9">
+        <v>46</v>
+      </c>
+      <c r="D153" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E153" s="10" t="s">
+        <v>16</v>
+      </c>
       <c r="F153" s="9"/>
       <c r="G153" s="9"/>
       <c r="H153" s="9"/>
       <c r="I153" s="9"/>
-      <c r="J153" s="9"/>
+      <c r="J153" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="K153" s="9"/>
-      <c r="L153" s="9"/>
-      <c r="M153" s="9"/>
+      <c r="L153" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M153" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A154" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B154" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C154" s="9">
+        <v>47</v>
+      </c>
+      <c r="D154" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="E154" s="10"/>
+      <c r="G154" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="J154" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="L154" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="M154" s="9" t="s">
+        <v>26</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
updated for completed tests
</commit_message>
<xml_diff>
--- a/validation/examples/reinsurance_test_case_list.xlsx
+++ b/validation/examples/reinsurance_test_case_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64_2\home\Joh\OasisLMF\validation\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys64\home\Joh\OasisLMF_branch\validation\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6ADD8C81-D4E2-4F91-AB77-0BDD3881E52D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94827CF5-0AC4-4BB6-ADF7-C0B75CF9B2BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{B6E553A6-C91A-4048-92DA-95C85460DBE0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$M$152</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,6 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -33,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="850" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="840" uniqueCount="26">
   <si>
     <t>FolderName</t>
   </si>
@@ -111,21 +114,6 @@
   </si>
   <si>
     <t>complete</t>
-  </si>
-  <si>
-    <t>in progress</t>
-  </si>
-  <si>
-    <t>13-19</t>
-  </si>
-  <si>
-    <t>16, 23</t>
-  </si>
-  <si>
-    <t>QS46_x6</t>
-  </si>
-  <si>
-    <t>QS47_x2</t>
   </si>
 </sst>
 </file>
@@ -518,33 +506,33 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FE6CEA-CC45-4060-BB7B-A215E1EF8A28}">
-  <dimension ref="A1:N154"/>
+  <dimension ref="A1:N155"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B120" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B138" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M154" sqref="M154"/>
+      <selection pane="bottomRight" activeCell="A150" sqref="A150:M153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.44140625" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="8" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.7109375" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.85546875" style="1"/>
+    <col min="11" max="11" width="8.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -585,7 +573,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="str">
         <f>LEFT(D2,2)&amp;TEXT(C2,"00")&amp;"_"&amp;B2</f>
         <v>SS01_1</v>
@@ -614,7 +602,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
         <f t="shared" ref="A3:A66" si="0">LEFT(D3,2)&amp;TEXT(C3,"00")&amp;"_"&amp;B3</f>
         <v>SS01_2</v>
@@ -647,7 +635,7 @@
       </c>
       <c r="N3" s="2"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS01_3</v>
@@ -676,7 +664,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_4</v>
@@ -708,7 +696,7 @@
       </c>
       <c r="M5" s="2"/>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_5</v>
@@ -739,7 +727,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS02_6</v>
@@ -774,7 +762,7 @@
       </c>
       <c r="N7" s="2"/>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_7</v>
@@ -809,7 +797,7 @@
       </c>
       <c r="N8" s="2"/>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_8</v>
@@ -840,7 +828,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS03_9</v>
@@ -872,7 +860,7 @@
       </c>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS04_10</v>
@@ -905,7 +893,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>SS04_11</v>
@@ -942,7 +930,7 @@
       </c>
       <c r="N12" s="2"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="str">
         <f t="shared" si="0"/>
         <v>SS04_12</v>
@@ -975,7 +963,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_13</v>
@@ -1004,7 +992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_14</v>
@@ -1033,7 +1021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_15</v>
@@ -1066,7 +1054,7 @@
       </c>
       <c r="N16" s="2"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS05_16</v>
@@ -1096,7 +1084,7 @@
       </c>
       <c r="N17" s="2"/>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_17</v>
@@ -1131,7 +1119,7 @@
       </c>
       <c r="N18" s="2"/>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_18</v>
@@ -1162,7 +1150,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS06_19</v>
@@ -1193,7 +1181,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_20</v>
@@ -1224,7 +1212,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_21</v>
@@ -1259,7 +1247,7 @@
       </c>
       <c r="N22" s="2"/>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_22</v>
@@ -1290,7 +1278,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS07_23</v>
@@ -1318,7 +1306,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_24</v>
@@ -1351,7 +1339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_25</v>
@@ -1384,7 +1372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS08_26</v>
@@ -1421,7 +1409,7 @@
       </c>
       <c r="N27" s="2"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_27</v>
@@ -1454,7 +1442,7 @@
       </c>
       <c r="N28" s="2"/>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_28</v>
@@ -1483,7 +1471,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_29</v>
@@ -1512,7 +1500,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS09_30</v>
@@ -1542,7 +1530,7 @@
       </c>
       <c r="N31" s="2"/>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A32" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_31</v>
@@ -1573,7 +1561,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_32</v>
@@ -1608,7 +1596,7 @@
       </c>
       <c r="N33" s="2"/>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A34" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS10_33</v>
@@ -1639,7 +1627,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A35" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_34</v>
@@ -1670,7 +1658,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A36" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_35</v>
@@ -1701,7 +1689,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A37" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_36</v>
@@ -1736,7 +1724,7 @@
       </c>
       <c r="N37" s="2"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS11_37</v>
@@ -1768,7 +1756,7 @@
       </c>
       <c r="N38" s="2"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_38</v>
@@ -1805,7 +1793,7 @@
       </c>
       <c r="N39" s="2"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A40" s="1" t="str">
         <f t="shared" si="0"/>
         <v>QS12_39</v>
@@ -1838,7 +1826,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A41" s="6" t="str">
         <f t="shared" si="0"/>
         <v>QS12_40</v>
@@ -1871,7 +1859,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A42" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_41</v>
@@ -1900,7 +1888,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A43" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_42</v>
@@ -1933,7 +1921,7 @@
       </c>
       <c r="N43" s="2"/>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_43</v>
@@ -1962,7 +1950,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A45" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR13_44</v>
@@ -1992,7 +1980,7 @@
       </c>
       <c r="N45" s="2"/>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A46" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_45</v>
@@ -2023,7 +2011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A47" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_46</v>
@@ -2054,7 +2042,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A48" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR14_47</v>
@@ -2089,7 +2077,7 @@
       </c>
       <c r="N48" s="2"/>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A49" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_48</v>
@@ -2124,7 +2112,7 @@
       </c>
       <c r="N49" s="2"/>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_49</v>
@@ -2155,7 +2143,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A51" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR15_50</v>
@@ -2186,7 +2174,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A52" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_51</v>
@@ -2219,7 +2207,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_52</v>
@@ -2256,7 +2244,7 @@
       </c>
       <c r="N53" s="2"/>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A54" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR16_53</v>
@@ -2289,7 +2277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A55" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_54</v>
@@ -2320,7 +2308,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A56" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_55</v>
@@ -2351,7 +2339,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A57" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_56</v>
@@ -2386,7 +2374,7 @@
       </c>
       <c r="N57" s="2"/>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A58" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR17_57</v>
@@ -2418,7 +2406,7 @@
       </c>
       <c r="N58" s="2"/>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A59" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_58</v>
@@ -2455,7 +2443,7 @@
       </c>
       <c r="N59" s="2"/>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A60" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR18_59</v>
@@ -2488,7 +2476,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A61" s="9" t="str">
         <f t="shared" si="0"/>
         <v>PR18_60</v>
@@ -2521,7 +2509,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A62" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_61</v>
@@ -2554,7 +2542,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A63" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_62</v>
@@ -2591,7 +2579,7 @@
       </c>
       <c r="N63" s="2"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A64" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR19_63</v>
@@ -2624,7 +2612,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_64</v>
@@ -2659,7 +2647,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A66" s="1" t="str">
         <f t="shared" si="0"/>
         <v>PR20_65</v>
@@ -2694,7 +2682,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A67" s="1" t="str">
         <f t="shared" ref="A67:A130" si="1">LEFT(D67,2)&amp;TEXT(C67,"00")&amp;"_"&amp;B67</f>
         <v>PR20_66</v>
@@ -2733,7 +2721,7 @@
       </c>
       <c r="N67" s="2"/>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A68" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_67</v>
@@ -2766,7 +2754,7 @@
       </c>
       <c r="N68" s="2"/>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A69" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_68</v>
@@ -2795,7 +2783,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_69</v>
@@ -2824,7 +2812,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A71" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR21_70</v>
@@ -2850,7 +2838,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A72" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_71</v>
@@ -2881,7 +2869,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A73" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_72</v>
@@ -2916,7 +2904,7 @@
       </c>
       <c r="N73" s="2"/>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A74" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR22_73</v>
@@ -2947,7 +2935,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A75" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_74</v>
@@ -2978,7 +2966,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_75</v>
@@ -3009,7 +2997,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A77" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR23_76</v>
@@ -3044,7 +3032,7 @@
       </c>
       <c r="N77" s="2"/>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A78" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_77</v>
@@ -3081,7 +3069,7 @@
       </c>
       <c r="N78" s="2"/>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A79" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_78</v>
@@ -3114,7 +3102,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A80" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR24_79</v>
@@ -3147,7 +3135,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A81" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_80</v>
@@ -3178,7 +3166,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A82" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_81</v>
@@ -3213,7 +3201,7 @@
       </c>
       <c r="N82" s="2"/>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A83" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_82</v>
@@ -3244,7 +3232,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A84" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR25_83</v>
@@ -3276,7 +3264,7 @@
       </c>
       <c r="N84" s="2"/>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A85" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_84</v>
@@ -3309,7 +3297,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A86" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR26_85</v>
@@ -3342,7 +3330,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A87" s="9" t="str">
         <f t="shared" si="1"/>
         <v>PR26_86</v>
@@ -3379,7 +3367,7 @@
       </c>
       <c r="N87" s="2"/>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A88" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_87</v>
@@ -3416,7 +3404,7 @@
       </c>
       <c r="N88" s="2"/>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A89" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_88</v>
@@ -3449,7 +3437,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A90" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR27_89</v>
@@ -3482,7 +3470,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A91" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_90</v>
@@ -3517,7 +3505,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A92" s="1" t="str">
         <f t="shared" si="1"/>
         <v>PR28_91</v>
@@ -3556,7 +3544,7 @@
       </c>
       <c r="N92" s="2"/>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A93" s="6" t="str">
         <f t="shared" si="1"/>
         <v>PR28_92</v>
@@ -3591,7 +3579,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A94" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_93</v>
@@ -3620,7 +3608,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A95" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_94</v>
@@ -3649,7 +3637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A96" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_95</v>
@@ -3682,7 +3670,7 @@
       </c>
       <c r="N96" s="2"/>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A97" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX29_96</v>
@@ -3712,7 +3700,7 @@
       </c>
       <c r="N97" s="2"/>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A98" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_97</v>
@@ -3747,7 +3735,7 @@
       </c>
       <c r="N98" s="2"/>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A99" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_98</v>
@@ -3778,7 +3766,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A100" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_99</v>
@@ -3809,7 +3797,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A101" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX30_100</v>
@@ -3841,7 +3829,7 @@
       </c>
       <c r="N101" s="2"/>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A102" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_101</v>
@@ -3872,7 +3860,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A103" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_102</v>
@@ -3907,7 +3895,7 @@
       </c>
       <c r="N103" s="2"/>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A104" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_103</v>
@@ -3938,7 +3926,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A105" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX31_104</v>
@@ -3970,7 +3958,7 @@
       </c>
       <c r="N105" s="2"/>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A106" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_105</v>
@@ -4003,7 +3991,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A107" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_106</v>
@@ -4036,7 +4024,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A108" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_107</v>
@@ -4073,7 +4061,7 @@
       </c>
       <c r="N108" s="2"/>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A109" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX32_108</v>
@@ -4107,7 +4095,7 @@
       </c>
       <c r="N109" s="2"/>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A110" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_109</v>
@@ -4136,10 +4124,10 @@
         <v>22</v>
       </c>
       <c r="M110" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="111" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A111" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_110</v>
@@ -4168,7 +4156,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A112" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_111</v>
@@ -4197,7 +4185,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A113" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX33_112</v>
@@ -4223,10 +4211,10 @@
         <v>22</v>
       </c>
       <c r="M113" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A114" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_113</v>
@@ -4257,7 +4245,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A115" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_114</v>
@@ -4288,10 +4276,10 @@
         <v>22</v>
       </c>
       <c r="M115" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A116" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_115</v>
@@ -4322,7 +4310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A117" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX34_116</v>
@@ -4350,10 +4338,10 @@
         <v>22</v>
       </c>
       <c r="M117" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A118" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_117</v>
@@ -4384,7 +4372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A119" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_118</v>
@@ -4415,7 +4403,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_119</v>
@@ -4446,10 +4434,10 @@
         <v>22</v>
       </c>
       <c r="M120" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX35_120</v>
@@ -4477,10 +4465,10 @@
         <v>22</v>
       </c>
       <c r="M121" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_121</v>
@@ -4513,10 +4501,10 @@
         <v>22</v>
       </c>
       <c r="M122" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_122</v>
@@ -4549,7 +4537,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="str">
         <f t="shared" si="1"/>
         <v>CX36_123</v>
@@ -4582,7 +4570,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A125" s="6" t="str">
         <f t="shared" si="1"/>
         <v>CX36_124</v>
@@ -4613,10 +4601,10 @@
         <v>22</v>
       </c>
       <c r="M125" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A126" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_125</v>
@@ -4649,7 +4637,7 @@
       </c>
       <c r="N126" s="2"/>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_126</v>
@@ -4678,7 +4666,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A128" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA37_127</v>
@@ -4707,7 +4695,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A129" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA38_128</v>
@@ -4738,7 +4726,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A130" s="1" t="str">
         <f t="shared" si="1"/>
         <v>FA38_129</v>
@@ -4773,7 +4761,7 @@
       </c>
       <c r="N130" s="2"/>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A131" s="1" t="str">
         <f t="shared" ref="A131:A149" si="2">LEFT(D131,2)&amp;TEXT(C131,"00")&amp;"_"&amp;B131</f>
         <v>FA38_130</v>
@@ -4804,7 +4792,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A132" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_131</v>
@@ -4835,7 +4823,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A133" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_132</v>
@@ -4866,7 +4854,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A134" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA39_133</v>
@@ -4901,7 +4889,7 @@
       </c>
       <c r="N134" s="2"/>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A135" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_134</v>
@@ -4938,7 +4926,7 @@
       </c>
       <c r="N135" s="2"/>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A136" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_135</v>
@@ -4971,7 +4959,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A137" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA40_136</v>
@@ -5004,7 +4992,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A138" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_137</v>
@@ -5033,7 +5021,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A139" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_138</v>
@@ -5066,7 +5054,7 @@
       </c>
       <c r="N139" s="2"/>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A140" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA41_139</v>
@@ -5095,7 +5083,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A141" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_140</v>
@@ -5126,7 +5114,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A142" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_141</v>
@@ -5157,7 +5145,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A143" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA42_142</v>
@@ -5192,7 +5180,7 @@
       </c>
       <c r="N143" s="2"/>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A144" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_143</v>
@@ -5227,7 +5215,7 @@
       </c>
       <c r="N144" s="2"/>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A145" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_144</v>
@@ -5258,7 +5246,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A146" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA43_145</v>
@@ -5289,7 +5277,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A147" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA44_146</v>
@@ -5322,7 +5310,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A148" s="1" t="str">
         <f t="shared" si="2"/>
         <v>FA44_147</v>
@@ -5359,7 +5347,7 @@
       </c>
       <c r="N148" s="2"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A149" s="9" t="str">
         <f t="shared" si="2"/>
         <v>FA44_148</v>
@@ -5393,9 +5381,9 @@
       </c>
       <c r="M149" s="9"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A150" s="9" t="str">
-        <f t="shared" ref="A150:A152" si="3">LEFT(D150,2)&amp;TEXT(C150,"00")&amp;"_"&amp;B150</f>
+        <f t="shared" ref="A150:A153" si="3">LEFT(D150,2)&amp;TEXT(C150,"00")&amp;"_"&amp;B150</f>
         <v>FA45_149</v>
       </c>
       <c r="B150" s="9">
@@ -5429,7 +5417,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A151" s="9" t="str">
         <f t="shared" si="3"/>
         <v>FA45_150</v>
@@ -5465,33 +5453,33 @@
         <v>25</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A152" s="6" t="str">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A152" s="9" t="str">
         <f t="shared" si="3"/>
         <v>FA45_151</v>
       </c>
-      <c r="B152" s="6">
+      <c r="B152" s="9">
         <v>151</v>
       </c>
-      <c r="C152" s="6">
+      <c r="C152" s="9">
         <v>45</v>
       </c>
-      <c r="D152" s="8" t="s">
+      <c r="D152" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="E152" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F152" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="G152" s="8"/>
-      <c r="H152" s="8"/>
-      <c r="I152" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="J152" s="6"/>
-      <c r="K152" s="6" t="s">
+      <c r="E152" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="F152" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G152" s="10"/>
+      <c r="H152" s="10"/>
+      <c r="I152" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="J152" s="9"/>
+      <c r="K152" s="9" t="s">
         <v>15</v>
       </c>
       <c r="L152" s="9" t="s">
@@ -5501,63 +5489,57 @@
         <v>25</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A153" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B153" s="9" t="s">
-        <v>27</v>
+    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A153" s="9" t="str">
+        <f t="shared" si="3"/>
+        <v>FA45_152</v>
+      </c>
+      <c r="B153" s="9">
+        <v>152</v>
       </c>
       <c r="C153" s="9">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D153" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="E153" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="F153" s="9"/>
-      <c r="G153" s="9"/>
-      <c r="H153" s="9"/>
-      <c r="I153" s="9"/>
-      <c r="J153" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="K153" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="E153" s="10"/>
+      <c r="F153" s="10"/>
+      <c r="G153" s="10"/>
+      <c r="H153" s="10"/>
+      <c r="I153" s="10"/>
+      <c r="J153" s="9"/>
+      <c r="K153" s="9" t="s">
+        <v>14</v>
+      </c>
       <c r="L153" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M153" s="9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A154" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="B154" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C154" s="9">
-        <v>47</v>
-      </c>
-      <c r="D154" s="10" t="s">
-        <v>17</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="M153" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A154" s="9"/>
+      <c r="B154" s="9"/>
+      <c r="C154" s="9"/>
+      <c r="D154" s="10"/>
       <c r="E154" s="10"/>
-      <c r="G154" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J154" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="L154" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="M154" s="9" t="s">
-        <v>26</v>
-      </c>
+      <c r="F154" s="9"/>
+      <c r="G154" s="9"/>
+      <c r="H154" s="9"/>
+      <c r="I154" s="9"/>
+      <c r="J154" s="9"/>
+      <c r="K154" s="9"/>
+      <c r="L154" s="9"/>
+      <c r="M154" s="9"/>
+    </row>
+    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="C155" s="9"/>
+      <c r="D155" s="10"/>
+      <c r="E155" s="10"/>
+      <c r="L155" s="9"/>
+      <c r="M155" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>